<commit_message>
Adding Parameter to method
</commit_message>
<xml_diff>
--- a/src/main/java/com/uktd/qa/testdata/AddAgent.xlsx
+++ b/src/main/java/com/uktd/qa/testdata/AddAgent.xlsx
@@ -4,25 +4,26 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="7935"/>
+    <workbookView windowWidth="19890" windowHeight="7935" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DataPool1" sheetId="1" r:id="rId1"/>
+    <sheet name="Datapool2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21">
-  <si>
-    <t>c_Name</t>
-  </si>
-  <si>
-    <t>p_Code</t>
-  </si>
-  <si>
-    <t>address</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29">
+  <si>
+    <t>m_Name</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>address1</t>
   </si>
   <si>
     <t>phNo</t>
@@ -77,6 +78,30 @@
   </si>
   <si>
     <t>www.testfive.com</t>
+  </si>
+  <si>
+    <t>R_Type</t>
+  </si>
+  <si>
+    <t>Purchase_Method</t>
+  </si>
+  <si>
+    <t>Application_Filling</t>
+  </si>
+  <si>
+    <t>Post_Code</t>
+  </si>
+  <si>
+    <t>Full Profile</t>
+  </si>
+  <si>
+    <t>Agent to Purchase</t>
+  </si>
+  <si>
+    <t>I want to enter the full details of applicant now</t>
+  </si>
+  <si>
+    <t>L118LZ</t>
   </si>
 </sst>
 </file>
@@ -85,8 +110,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
@@ -115,6 +140,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -123,14 +156,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -145,6 +170,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -168,15 +208,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -198,6 +230,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -206,34 +259,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -257,12 +282,66 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -275,43 +354,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -323,121 +396,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -448,6 +473,26 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -462,26 +507,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -511,21 +536,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -548,153 +558,168 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1035,8 +1060,8 @@
   <sheetPr/>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="5"/>
@@ -1140,4 +1165,55 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="11.4285714285714" customWidth="1"/>
+    <col min="2" max="2" width="18.5714285714286" customWidth="1"/>
+    <col min="3" max="3" width="47.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="11.1428571428571" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Up to Step 1 DDT done
</commit_message>
<xml_diff>
--- a/src/main/java/com/uktd/qa/testdata/AddAgent.xlsx
+++ b/src/main/java/com/uktd/qa/testdata/AddAgent.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19890" windowHeight="7935" activeTab="1"/>
+    <workbookView windowWidth="20385" windowHeight="7935" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DataPool1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68">
   <si>
     <t>m_Name</t>
   </si>
@@ -80,16 +80,76 @@
     <t>www.testfive.com</t>
   </si>
   <si>
-    <t>R_Type</t>
-  </si>
-  <si>
-    <t>Purchase_Method</t>
-  </si>
-  <si>
-    <t>Application_Filling</t>
-  </si>
-  <si>
-    <t>Post_Code</t>
+    <t>ReportType</t>
+  </si>
+  <si>
+    <t>PurchaseMethod</t>
+  </si>
+  <si>
+    <t>ApplicationFilling</t>
+  </si>
+  <si>
+    <t>PostCode</t>
+  </si>
+  <si>
+    <t>ApplicationAddress</t>
+  </si>
+  <si>
+    <t>MoveIndate</t>
+  </si>
+  <si>
+    <t>TenancyPeriod</t>
+  </si>
+  <si>
+    <t>MonthlyRent</t>
+  </si>
+  <si>
+    <t>RentShare</t>
+  </si>
+  <si>
+    <t>ApplicantTitle</t>
+  </si>
+  <si>
+    <t>ApplicantName</t>
+  </si>
+  <si>
+    <t>ApplicantMiddleName</t>
+  </si>
+  <si>
+    <t>ApplicantSurName</t>
+  </si>
+  <si>
+    <t>ApplicantMaidenName</t>
+  </si>
+  <si>
+    <t>ApplicantDOB</t>
+  </si>
+  <si>
+    <t>ApplicantMariatalStatus</t>
+  </si>
+  <si>
+    <t>HomePhone</t>
+  </si>
+  <si>
+    <t>WorkPhone</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>ConfirmEmail</t>
+  </si>
+  <si>
+    <t>Proof</t>
+  </si>
+  <si>
+    <t>NoOfChild</t>
+  </si>
+  <si>
+    <t>Child18+</t>
   </si>
   <si>
     <t>Full Profile</t>
@@ -102,6 +162,64 @@
   </si>
   <si>
     <t>L118LZ</t>
+  </si>
+  <si>
+    <t>30 Broad Lane Norris Green Liverpool</t>
+  </si>
+  <si>
+    <t>28/02/2019</t>
+  </si>
+  <si>
+    <t>24 months</t>
+  </si>
+  <si>
+    <t>18000</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>Mr</t>
+  </si>
+  <si>
+    <t>Sagar</t>
+  </si>
+  <si>
+    <t>Kisan</t>
+  </si>
+  <si>
+    <t>Mohite</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>28/01/1994</t>
+  </si>
+  <si>
+    <t>Married</t>
+  </si>
+  <si>
+    <t>02425261552</t>
+  </si>
+  <si>
+    <t>0202255881</t>
+  </si>
+  <si>
+    <t>9604328562</t>
+  </si>
+  <si>
+    <t xml:space="preserve">swapnilbhaskar@benchmarkitsolutions.com
+</t>
+  </si>
+  <si>
+    <t>Passport</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -110,8 +228,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
@@ -140,22 +258,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -170,45 +288,31 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -222,30 +326,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -259,7 +349,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -282,6 +400,144 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -294,175 +550,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -473,26 +591,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -507,6 +605,26 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -536,6 +654,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -558,27 +691,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -596,136 +714,139 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
@@ -1074,22 +1195,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1103,13 +1224,13 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1123,13 +1244,13 @@
       <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1143,13 +1264,13 @@
       <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1170,21 +1291,38 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="11.4285714285714" customWidth="1"/>
     <col min="2" max="2" width="18.5714285714286" customWidth="1"/>
     <col min="3" max="3" width="47.1428571428571" customWidth="1"/>
     <col min="4" max="4" width="11.1428571428571" customWidth="1"/>
+    <col min="5" max="5" width="37.1428571428571" customWidth="1"/>
+    <col min="6" max="6" width="12.5714285714286" customWidth="1"/>
+    <col min="7" max="7" width="15.2857142857143" customWidth="1"/>
+    <col min="8" max="8" width="13.5714285714286" customWidth="1"/>
+    <col min="9" max="9" width="10.8571428571429" customWidth="1"/>
+    <col min="10" max="10" width="14.4285714285714" customWidth="1"/>
+    <col min="11" max="11" width="16" customWidth="1"/>
+    <col min="12" max="12" width="23" customWidth="1"/>
+    <col min="13" max="13" width="19.1428571428571" customWidth="1"/>
+    <col min="14" max="14" width="23.4285714285714" customWidth="1"/>
+    <col min="15" max="15" width="14.2857142857143" customWidth="1"/>
+    <col min="16" max="16" width="24.2857142857143" customWidth="1"/>
+    <col min="17" max="17" width="12.8571428571429" customWidth="1"/>
+    <col min="18" max="18" width="12.2857142857143" customWidth="1"/>
+    <col min="19" max="19" width="11.7142857142857" customWidth="1"/>
+    <col min="20" max="20" width="39.8571428571429" customWidth="1"/>
+    <col min="21" max="21" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:24">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -1197,22 +1335,146 @@
       <c r="D1" t="s">
         <v>24</v>
       </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S1" t="s">
+        <v>39</v>
+      </c>
+      <c r="T1" t="s">
+        <v>40</v>
+      </c>
+      <c r="U1" t="s">
+        <v>41</v>
+      </c>
+      <c r="V1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W1" t="s">
+        <v>43</v>
+      </c>
+      <c r="X1" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" ht="18" customHeight="1" spans="1:24">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>48</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K2" t="s">
+        <v>55</v>
+      </c>
+      <c r="L2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M2" t="s">
+        <v>57</v>
+      </c>
+      <c r="N2" t="s">
+        <v>58</v>
+      </c>
+      <c r="O2" t="s">
+        <v>59</v>
+      </c>
+      <c r="P2" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="V2" t="s">
+        <v>65</v>
+      </c>
+      <c r="W2" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="X2" s="5" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="T2" r:id="rId1" display="swapnilbhaskar@benchmarkitsolutions.com&#10;"/>
+    <hyperlink ref="U2" r:id="rId1" display="swapnilbhaskar@benchmarkitsolutions.com&#10;"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
Step 5 successfully Added
</commit_message>
<xml_diff>
--- a/src/main/java/com/uktd/qa/testdata/AddAgent.xlsx
+++ b/src/main/java/com/uktd/qa/testdata/AddAgent.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19890" windowHeight="7935" activeTab="1"/>
+    <workbookView windowWidth="12720" windowHeight="5340" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DataPool1" sheetId="1" r:id="rId1"/>
     <sheet name="F&amp;F-Yes-LA&amp;Unemployed" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
+  <oleSize ref="A1:BL2"/>
 </workbook>
 </file>
 
@@ -511,67 +512,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -607,6 +550,64 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -623,187 +624,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -867,6 +868,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -890,36 +915,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -937,130 +938,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1519,7 +1520,7 @@
   <sheetPr/>
   <dimension ref="A1:BL2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BB1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="BM8" sqref="BM8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Entire XML suit completed
</commit_message>
<xml_diff>
--- a/src/main/java/com/uktd/qa/testdata/AddAgent.xlsx
+++ b/src/main/java/com/uktd/qa/testdata/AddAgent.xlsx
@@ -4,20 +4,22 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="7935" activeTab="2"/>
+    <workbookView windowWidth="20385" windowHeight="7935" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="DataPool1" sheetId="1" r:id="rId1"/>
     <sheet name="AgToPurAgFill&gt;F&amp;F-Yes-LA&amp;Unemp" sheetId="2" r:id="rId2"/>
     <sheet name="TenToPurTenFill&gt;F&amp;F-Yes-LL&amp;Emp" sheetId="3" r:id="rId3"/>
+    <sheet name="AgToPurAgFillCR" sheetId="4" r:id="rId4"/>
+    <sheet name="TenPurTenFillCR" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <oleSize ref="R1:CC2"/>
+  <oleSize ref="S1:CD2"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194">
   <si>
     <t>m_Name</t>
   </si>
@@ -247,10 +249,10 @@
     <t>KinYOK</t>
   </si>
   <si>
+    <t>InsuranceNo</t>
+  </si>
+  <si>
     <t>EmpType</t>
-  </si>
-  <si>
-    <t>InsuranceNo</t>
   </si>
   <si>
     <t>FamilyTaxCredit</t>
@@ -426,12 +428,12 @@
     <t>5</t>
   </si>
   <si>
+    <t>IND2018</t>
+  </si>
+  <si>
     <t>Unemployed</t>
   </si>
   <si>
-    <t>IND2018</t>
-  </si>
-  <si>
     <t>200</t>
   </si>
   <si>
@@ -580,6 +582,27 @@
   </si>
   <si>
     <t>1500</t>
+  </si>
+  <si>
+    <t>Credit Report Only</t>
+  </si>
+  <si>
+    <t>Sumit</t>
+  </si>
+  <si>
+    <t>Karan</t>
+  </si>
+  <si>
+    <t>Kumar</t>
+  </si>
+  <si>
+    <t>26 Broad Lane Norris Green Liverpool</t>
+  </si>
+  <si>
+    <t>Mayur</t>
+  </si>
+  <si>
+    <t>Mane</t>
   </si>
 </sst>
 </file>
@@ -588,8 +611,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
@@ -618,14 +641,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -640,25 +655,18 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -686,7 +694,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -708,10 +724,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -723,17 +740,16 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -744,6 +760,13 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -760,7 +783,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -772,31 +843,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -808,37 +897,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -850,31 +927,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -886,61 +957,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -951,26 +974,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -985,6 +988,26 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1014,6 +1037,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -1036,27 +1074,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1074,130 +1097,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1656,8 +1679,8 @@
   <sheetPr/>
   <dimension ref="A1:BL2"/>
   <sheetViews>
-    <sheetView topLeftCell="AZ1" workbookViewId="0">
-      <selection activeCell="BE24" sqref="BE24"/>
+    <sheetView topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1:X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -2125,8 +2148,8 @@
   <sheetPr/>
   <dimension ref="A1:BZ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="W15" sqref="W15"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -2364,7 +2387,7 @@
         <v>151</v>
       </c>
       <c r="BE1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="BF1" t="s">
         <v>152</v>
@@ -2597,7 +2620,7 @@
         <v>134</v>
       </c>
       <c r="BD2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="BE2" t="s">
         <v>175</v>
@@ -2676,4 +2699,453 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:AC2"/>
+  <sheetViews>
+    <sheetView topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1:AC2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="18.5714285714286" customWidth="1"/>
+    <col min="3" max="3" width="47.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="37.1428571428571" customWidth="1"/>
+    <col min="6" max="6" width="12.5714285714286" customWidth="1"/>
+    <col min="7" max="7" width="15.2857142857143" customWidth="1"/>
+    <col min="8" max="8" width="13.5714285714286" customWidth="1"/>
+    <col min="15" max="15" width="14.2857142857143" customWidth="1"/>
+    <col min="17" max="17" width="12.8571428571429" customWidth="1"/>
+    <col min="18" max="18" width="12.2857142857143" customWidth="1"/>
+    <col min="19" max="19" width="11.7142857142857" customWidth="1"/>
+    <col min="20" max="20" width="40.2857142857143" customWidth="1"/>
+    <col min="21" max="21" width="40.7142857142857" customWidth="1"/>
+    <col min="23" max="23" width="9.42857142857143" customWidth="1"/>
+    <col min="24" max="24" width="10.1428571428571" customWidth="1"/>
+    <col min="25" max="25" width="17.5714285714286" customWidth="1"/>
+    <col min="26" max="26" width="45.7142857142857" customWidth="1"/>
+    <col min="27" max="27" width="19.5714285714286" customWidth="1"/>
+    <col min="28" max="28" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S1" t="s">
+        <v>39</v>
+      </c>
+      <c r="T1" t="s">
+        <v>40</v>
+      </c>
+      <c r="U1" t="s">
+        <v>41</v>
+      </c>
+      <c r="V1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W1" t="s">
+        <v>64</v>
+      </c>
+      <c r="X1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" ht="30" spans="1:29">
+      <c r="A2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K2" t="s">
+        <v>188</v>
+      </c>
+      <c r="L2" t="s">
+        <v>189</v>
+      </c>
+      <c r="M2" t="s">
+        <v>190</v>
+      </c>
+      <c r="N2" t="s">
+        <v>97</v>
+      </c>
+      <c r="O2" t="s">
+        <v>98</v>
+      </c>
+      <c r="P2" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="V2" t="s">
+        <v>104</v>
+      </c>
+      <c r="W2" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="X2" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB2" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="AC2" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="T2" r:id="rId1" display="swapnilbhaskar@benchmarkitsolutions.com&#10;"/>
+    <hyperlink ref="U2" r:id="rId1" display="swapnilbhaskar@benchmarkitsolutions.com&#10;"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:AC2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AC11" sqref="AC11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="19.4285714285714" customWidth="1"/>
+    <col min="3" max="3" width="51.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="37.1428571428571" customWidth="1"/>
+    <col min="6" max="6" width="12.5714285714286" customWidth="1"/>
+    <col min="7" max="7" width="15.2857142857143" customWidth="1"/>
+    <col min="8" max="8" width="13.5714285714286" customWidth="1"/>
+    <col min="9" max="9" width="10.8571428571429" customWidth="1"/>
+    <col min="10" max="10" width="14.4285714285714" customWidth="1"/>
+    <col min="11" max="11" width="16" customWidth="1"/>
+    <col min="12" max="12" width="19.1428571428571" customWidth="1"/>
+    <col min="13" max="13" width="11.7142857142857" customWidth="1"/>
+    <col min="14" max="14" width="41" customWidth="1"/>
+    <col min="15" max="15" width="39.8571428571429" customWidth="1"/>
+    <col min="16" max="16" width="23" customWidth="1"/>
+    <col min="17" max="17" width="23.4285714285714" customWidth="1"/>
+    <col min="18" max="18" width="14.2857142857143" customWidth="1"/>
+    <col min="19" max="19" width="24.2857142857143" customWidth="1"/>
+    <col min="20" max="20" width="12.8571428571429" customWidth="1"/>
+    <col min="21" max="21" width="12.2857142857143" customWidth="1"/>
+    <col min="23" max="23" width="9.42857142857143" customWidth="1"/>
+    <col min="24" max="24" width="10.1428571428571" customWidth="1"/>
+    <col min="25" max="25" width="17.5714285714286" customWidth="1"/>
+    <col min="26" max="26" width="45.7142857142857" customWidth="1"/>
+    <col min="27" max="27" width="19.5714285714286" customWidth="1"/>
+    <col min="28" max="28" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S1" t="s">
+        <v>36</v>
+      </c>
+      <c r="T1" t="s">
+        <v>37</v>
+      </c>
+      <c r="U1" t="s">
+        <v>38</v>
+      </c>
+      <c r="V1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W1" t="s">
+        <v>64</v>
+      </c>
+      <c r="X1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" ht="30" spans="1:29">
+      <c r="A2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" t="s">
+        <v>191</v>
+      </c>
+      <c r="F2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K2" t="s">
+        <v>192</v>
+      </c>
+      <c r="L2" t="s">
+        <v>193</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="P2" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>97</v>
+      </c>
+      <c r="R2" t="s">
+        <v>98</v>
+      </c>
+      <c r="S2" t="s">
+        <v>99</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="V2" t="s">
+        <v>104</v>
+      </c>
+      <c r="W2" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="X2" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB2" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="AC2" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="N2" r:id="rId1" display="swapnilbhaskar@benchmarkitsolutions.com&#10;"/>
+    <hyperlink ref="O2" r:id="rId1" display="swapnilbhaskar@benchmarkitsolutions.com&#10;"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
EmploymenT and Acc Check done
</commit_message>
<xml_diff>
--- a/src/main/java/com/uktd/qa/testdata/AddAgent.xlsx
+++ b/src/main/java/com/uktd/qa/testdata/AddAgent.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="7935" firstSheet="2" activeTab="5"/>
+    <workbookView windowWidth="20385" windowHeight="7935" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="DataPool1" sheetId="1" r:id="rId1"/>
@@ -12,15 +12,17 @@
     <sheet name="TenToPurTenFill&gt;F&amp;F-Yes-LL&amp;Emp" sheetId="3" r:id="rId3"/>
     <sheet name="AgToPurAgFillCR" sheetId="4" r:id="rId4"/>
     <sheet name="TenPurTenFillCR" sheetId="5" r:id="rId5"/>
-    <sheet name="LA&amp;EmpRefCheck" sheetId="6" r:id="rId6"/>
+    <sheet name="LA&amp;EmpRefCheck" sheetId="6" state="hidden" r:id="rId6"/>
+    <sheet name="LL&amp;SelfEmpRefCheck" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <oleSize ref="P1:CA2"/>
+  <oleSize ref="A1:BL2"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228">
   <si>
     <t>m_Name</t>
   </si>
@@ -622,6 +624,90 @@
   </si>
   <si>
     <t>Currently Renting</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>BusinessName</t>
+  </si>
+  <si>
+    <t>YearsofTrade</t>
+  </si>
+  <si>
+    <t>Businesstype</t>
+  </si>
+  <si>
+    <t>Jobtitle</t>
+  </si>
+  <si>
+    <t>AnnIncome</t>
+  </si>
+  <si>
+    <t>AnnBonus</t>
+  </si>
+  <si>
+    <t>Acctitle</t>
+  </si>
+  <si>
+    <t>AccFName</t>
+  </si>
+  <si>
+    <t>AccLName</t>
+  </si>
+  <si>
+    <t>AccPractName</t>
+  </si>
+  <si>
+    <t>OfficePCode</t>
+  </si>
+  <si>
+    <t>OfficeAddress</t>
+  </si>
+  <si>
+    <t>OfficeEmail</t>
+  </si>
+  <si>
+    <t>OfficePhone</t>
+  </si>
+  <si>
+    <t>OfficeMobile</t>
+  </si>
+  <si>
+    <t>OfficeFax</t>
+  </si>
+  <si>
+    <t>Self-Employed / Director of own company</t>
+  </si>
+  <si>
+    <t>WallMart</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>ShoppingCenter</t>
+  </si>
+  <si>
+    <t>Sales Officer</t>
+  </si>
+  <si>
+    <t>254800</t>
+  </si>
+  <si>
+    <t>25000</t>
+  </si>
+  <si>
+    <t>Romi</t>
+  </si>
+  <si>
+    <t>Singh</t>
+  </si>
+  <si>
+    <t>Rachel</t>
+  </si>
+  <si>
+    <t>01234567</t>
   </si>
 </sst>
 </file>
@@ -630,8 +716,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
@@ -660,6 +746,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -674,18 +768,25 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -713,15 +814,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -743,23 +836,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -772,10 +857,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -802,19 +888,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -844,19 +948,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -868,37 +1002,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -916,43 +1050,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -964,25 +1068,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -993,6 +1079,26 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1007,26 +1113,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1056,21 +1142,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -1093,153 +1164,168 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1698,8 +1784,8 @@
   <sheetPr/>
   <dimension ref="A1:BL2"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="V1" sqref="$A1:$XFD1048576"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -2167,8 +2253,8 @@
   <sheetPr/>
   <dimension ref="A1:BZ2"/>
   <sheetViews>
-    <sheetView topLeftCell="BD1" workbookViewId="0">
-      <selection activeCell="BD1" sqref="BD1"/>
+    <sheetView topLeftCell="BQ1" workbookViewId="0">
+      <selection activeCell="CA5" sqref="CA5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -2947,7 +3033,7 @@
   <dimension ref="A1:AC2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AC11" sqref="AC11"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -3172,13 +3258,13 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:BW2"/>
+  <dimension ref="A1:BW14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView topLeftCell="BO1" workbookViewId="0">
+      <selection activeCell="CB17" sqref="CB17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.4285714285714" customWidth="1"/>
     <col min="2" max="2" width="18.5714285714286" customWidth="1"/>
@@ -3703,6 +3789,1015 @@
         <v>141</v>
       </c>
     </row>
+    <row r="14" spans="5:5">
+      <c r="E14" t="s">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="T2" r:id="rId1" display="swapnilbhaskar@benchmarkitsolutions.com&#10;"/>
+    <hyperlink ref="U2" r:id="rId1" display="swapnilbhaskar@benchmarkitsolutions.com&#10;"/>
+    <hyperlink ref="BM2" r:id="rId2" display="swapnilbhaskar@benchmarkitsolutions.com" tooltip="mailto:swapnilbhaskar@benchmarkitsolutions.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:BX2"/>
+  <sheetViews>
+    <sheetView topLeftCell="BP1" workbookViewId="0">
+      <selection activeCell="BT18" sqref="BT18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
+  <cols>
+    <col min="20" max="20" width="40" customWidth="1"/>
+    <col min="21" max="21" width="40.1428571428571" customWidth="1"/>
+    <col min="25" max="25" width="20" customWidth="1"/>
+    <col min="27" max="27" width="45.7142857142857" customWidth="1"/>
+    <col min="28" max="28" width="19.5714285714286" customWidth="1"/>
+    <col min="37" max="37" width="37" customWidth="1"/>
+    <col min="48" max="48" width="11.7142857142857" customWidth="1"/>
+    <col min="49" max="49" width="37.5714285714286" customWidth="1"/>
+    <col min="52" max="52" width="13" customWidth="1"/>
+    <col min="53" max="53" width="42" customWidth="1"/>
+    <col min="54" max="54" width="15.1428571428571" customWidth="1"/>
+    <col min="56" max="56" width="16.5714285714286" customWidth="1"/>
+    <col min="57" max="57" width="12.5714285714286" customWidth="1"/>
+    <col min="58" max="58" width="11.4285714285714" customWidth="1"/>
+    <col min="59" max="59" width="11.8571428571429" customWidth="1"/>
+    <col min="60" max="60" width="10.5714285714286" customWidth="1"/>
+    <col min="62" max="62" width="11" customWidth="1"/>
+    <col min="63" max="63" width="10.8571428571429" customWidth="1"/>
+    <col min="64" max="64" width="14.8571428571429" customWidth="1"/>
+    <col min="65" max="65" width="13" customWidth="1"/>
+    <col min="66" max="66" width="46.8571428571429" customWidth="1"/>
+    <col min="67" max="67" width="42.8571428571429" customWidth="1"/>
+    <col min="68" max="68" width="13" customWidth="1"/>
+    <col min="71" max="71" width="16.5714285714286" customWidth="1"/>
+    <col min="72" max="72" width="16.2857142857143" customWidth="1"/>
+    <col min="73" max="73" width="16.7142857142857" customWidth="1"/>
+    <col min="74" max="74" width="19.5714285714286" customWidth="1"/>
+    <col min="75" max="75" width="13.4285714285714" customWidth="1"/>
+    <col min="76" max="76" width="11.1428571428571" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:76">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S1" t="s">
+        <v>39</v>
+      </c>
+      <c r="T1" t="s">
+        <v>40</v>
+      </c>
+      <c r="U1" t="s">
+        <v>41</v>
+      </c>
+      <c r="V1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W1" t="s">
+        <v>43</v>
+      </c>
+      <c r="X1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>149</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>77</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>201</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>202</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>203</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>204</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>164</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>205</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>206</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>207</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>208</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>210</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>211</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>212</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>213</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>215</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>216</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>80</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>81</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>82</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" ht="30" spans="1:76">
+      <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K2" t="s">
+        <v>94</v>
+      </c>
+      <c r="L2" t="s">
+        <v>95</v>
+      </c>
+      <c r="M2" t="s">
+        <v>96</v>
+      </c>
+      <c r="N2" t="s">
+        <v>97</v>
+      </c>
+      <c r="O2" t="s">
+        <v>98</v>
+      </c>
+      <c r="P2" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="V2" t="s">
+        <v>104</v>
+      </c>
+      <c r="W2" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="X2" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>199</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE2" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>173</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>174</v>
+      </c>
+      <c r="AI2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="AJ2" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="AK2" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="AL2" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>123</v>
+      </c>
+      <c r="AN2" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="AO2" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>126</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>129</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>130</v>
+      </c>
+      <c r="AU2" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="AV2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="AW2" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>133</v>
+      </c>
+      <c r="AY2" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>135</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>217</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>218</v>
+      </c>
+      <c r="BC2" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>220</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>221</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>109</v>
+      </c>
+      <c r="BG2" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="BH2" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>116</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>224</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>225</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>226</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>7</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>8</v>
+      </c>
+      <c r="BO2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="BP2" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="BQ2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="BR2" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="BS2" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="BT2" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="BU2" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="BV2" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="BW2" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="T2" r:id="rId1" display="swapnilbhaskar@benchmarkitsolutions.com&#10;"/>
+    <hyperlink ref="U2" r:id="rId1" display="swapnilbhaskar@benchmarkitsolutions.com&#10;"/>
+    <hyperlink ref="AK2" r:id="rId2" display="amitbaghel@benchmarkitsolutions.com"/>
+    <hyperlink ref="BO2" r:id="rId1" display="swapnilbhaskar@benchmarkitsolutions.com&#10;"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:BW2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="12.1428571428571" customWidth="1"/>
+    <col min="2" max="2" width="18.5714285714286" customWidth="1"/>
+    <col min="3" max="3" width="47.1428571428571" customWidth="1"/>
+    <col min="5" max="5" width="37.1428571428571" customWidth="1"/>
+    <col min="6" max="6" width="12.5714285714286" customWidth="1"/>
+    <col min="7" max="7" width="15.2857142857143" customWidth="1"/>
+    <col min="8" max="8" width="13.5714285714286" customWidth="1"/>
+    <col min="20" max="20" width="40.1428571428571" customWidth="1"/>
+    <col min="21" max="21" width="39.8571428571429" customWidth="1"/>
+    <col min="25" max="25" width="20" customWidth="1"/>
+    <col min="38" max="38" width="41.1428571428571" customWidth="1"/>
+    <col min="50" max="50" width="36.4285714285714" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:75">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S1" t="s">
+        <v>39</v>
+      </c>
+      <c r="T1" t="s">
+        <v>40</v>
+      </c>
+      <c r="U1" t="s">
+        <v>41</v>
+      </c>
+      <c r="V1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W1" t="s">
+        <v>43</v>
+      </c>
+      <c r="X1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>77</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>152</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>153</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>154</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>155</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>157</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>158</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>159</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>160</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>161</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>162</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>163</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>164</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>165</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>166</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>80</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>81</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>82</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" ht="30" spans="1:75">
+      <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" t="s">
+        <v>195</v>
+      </c>
+      <c r="F2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K2" t="s">
+        <v>196</v>
+      </c>
+      <c r="L2" t="s">
+        <v>197</v>
+      </c>
+      <c r="M2" t="s">
+        <v>198</v>
+      </c>
+      <c r="N2" t="s">
+        <v>97</v>
+      </c>
+      <c r="O2" t="s">
+        <v>98</v>
+      </c>
+      <c r="P2" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="V2" t="s">
+        <v>104</v>
+      </c>
+      <c r="W2" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="X2" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>199</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AF2" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AJ2" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="AK2" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>121</v>
+      </c>
+      <c r="AM2" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>123</v>
+      </c>
+      <c r="AO2" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="AP2" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>126</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>129</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>130</v>
+      </c>
+      <c r="AV2" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="AW2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="AX2" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>133</v>
+      </c>
+      <c r="AZ2" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>135</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>177</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>178</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>179</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>7</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>180</v>
+      </c>
+      <c r="BG2" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="BH2" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>116</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>182</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>183</v>
+      </c>
+      <c r="BL2" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="BM2" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>179</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>186</v>
+      </c>
+      <c r="BP2" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="BQ2" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="BR2" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="BS2" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="BT2" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="BU2" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="BV2" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>141</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="T2" r:id="rId1" display="swapnilbhaskar@benchmarkitsolutions.com&#10;"/>

</xml_diff>